<commit_message>
Merged updated excel files into folders
</commit_message>
<xml_diff>
--- a/Battery_Capacity/Battery_Capacity.xlsx
+++ b/Battery_Capacity/Battery_Capacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/lcalimlim3_gatech_edu/Documents/Documents/ASE 6002 Portable Kettle/Battery_Capacity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/rgarcia46_gatech_edu/Documents/Documents/ASE6002/TA2/ASE6002PEK-main/ASE6002PEK-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{B39C7B50-4E94-4FA5-9D43-E848027EAA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3051A9D2-FCA4-4062-AF06-23EB9A5B4957}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{B39C7B50-4E94-4FA5-9D43-E848027EAA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FC4F333-B63A-4791-A702-E944486A0516}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="750" windowWidth="21570" windowHeight="11295" xr2:uid="{21964307-0BB7-4DE0-BD23-E82C9EC81DDB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{21964307-0BB7-4DE0-BD23-E82C9EC81DDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,10 +73,10 @@
     <t>J</t>
   </si>
   <si>
-    <t>"=capacity(mAh)*11.1(Vnominal)*36000(sec/hour)</t>
-  </si>
-  <si>
     <t>Battery_Capacity</t>
+  </si>
+  <si>
+    <t>"=capacity(Ah)*11.1(Vnominal)*36000(sec/hour)</t>
   </si>
 </sst>
 </file>
@@ -112,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,13 +452,13 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -469,7 +470,7 @@
       <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -489,7 +490,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <f>B3*3</f>
+        <f>Pack_Count*3</f>
         <v>9</v>
       </c>
       <c r="C4" t="s">
@@ -498,17 +499,17 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <f>B3*5000*11.1*3600</f>
-        <v>599400000</v>
+        <f>Pack_Count*5*11.1*3600</f>
+        <v>599400</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -516,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <f>B3*3*69</f>
+        <f>Pack_Count*3*69</f>
         <v>621</v>
       </c>
       <c r="C6" t="s">

</xml_diff>

<commit_message>
Add Uncertainty to Model
</commit_message>
<xml_diff>
--- a/Battery_Capacity/Battery_Capacity.xlsx
+++ b/Battery_Capacity/Battery_Capacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07531a99d7244c5b/Documents/GitHub/ASE6002PEK/Battery_Capacity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/lcalimlim3_gatech_edu/Documents/Documents/GitHub/ASE6002PEK/Battery_Capacity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{B39C7B50-4E94-4FA5-9D43-E848027EAA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCEE3B7E-792A-4D84-B2AB-74F8F9664314}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{B39C7B50-4E94-4FA5-9D43-E848027EAA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F167B64-A276-4F41-8E43-464F22E3454D}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="5430" windowWidth="38700" windowHeight="15345" xr2:uid="{21964307-0BB7-4DE0-BD23-E82C9EC81DDB}"/>
+    <workbookView xWindow="6345" yWindow="1125" windowWidth="21570" windowHeight="11295" xr2:uid="{21964307-0BB7-4DE0-BD23-E82C9EC81DDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="Cell_Count">Sheet1!$B$4</definedName>
     <definedName name="Cell_Weight">Sheet1!$B$6</definedName>
     <definedName name="Pack_Count">Sheet1!$B$3</definedName>
+    <definedName name="UNC_Batt_Cap">Sheet1!$B$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Battery Capacity</t>
   </si>
@@ -80,6 +81,12 @@
   </si>
   <si>
     <t>Battery_Cost</t>
+  </si>
+  <si>
+    <t>UNC_Batt_Cap</t>
+  </si>
+  <si>
+    <t>% Battery Carged</t>
   </si>
 </sst>
 </file>
@@ -455,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41EFFC3E-008D-46FD-8D1C-98A380E1D447}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,8 +515,8 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <f>Pack_Count*5*11.1*3600</f>
-        <v>599400</v>
+        <f>Pack_Count*5*11.1*3600*UNC_Batt_Cap</f>
+        <v>455544</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -537,6 +544,17 @@
       <c r="B7">
         <f>3.15*3*B3</f>
         <v>28.349999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added connection between cost and demand
Added variable and fixed costs to connect to demand model.
</commit_message>
<xml_diff>
--- a/Battery_Capacity/Battery_Capacity.xlsx
+++ b/Battery_Capacity/Battery_Capacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/lcalimlim3_gatech_edu/Documents/Documents/GitHub/ASE6002PEK/Battery_Capacity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07531a99d7244c5b/Documents/GitHub/ASE6002PEK/Battery_Capacity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="8_{B39C7B50-4E94-4FA5-9D43-E848027EAA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F167B64-A276-4F41-8E43-464F22E3454D}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{B39C7B50-4E94-4FA5-9D43-E848027EAA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F18F8C4-16CF-472E-82B7-67978A0BA908}"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="1125" windowWidth="21570" windowHeight="11295" xr2:uid="{21964307-0BB7-4DE0-BD23-E82C9EC81DDB}"/>
+    <workbookView xWindow="9105" yWindow="5325" windowWidth="38700" windowHeight="15345" xr2:uid="{21964307-0BB7-4DE0-BD23-E82C9EC81DDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -139,10 +139,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>